<commit_message>
Try to synch with my laptop
</commit_message>
<xml_diff>
--- a/HawkinsDaarud2019_Uncertainty/ds_cci.18.00066.xlsx
+++ b/HawkinsDaarud2019_Uncertainty/ds_cci.18.00066.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniofnottm-my.sharepoint.com/personal/nicholas_harbour_nottingham_ac_uk/Documents/Desktop/CMMB_Journal_club/HawkinsDaarud2019_Uncertainty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{8D3EBD06-EA18-42EC-91E7-F777F09A5E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CEBCA8C-54B6-4E03-8E89-1BCE225FEB31}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{8D3EBD06-EA18-42EC-91E7-F777F09A5E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D3C3FDD-F9D7-4A42-ACD2-E1C6732D9E21}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A0BC7E42-40D0-534B-A134-7DC0491EBAF1}"/>
+    <workbookView minimized="1" xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" xr2:uid="{A0BC7E42-40D0-534B-A134-7DC0491EBAF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -414,17 +414,23 @@
   <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="10.875" style="1"/>
-    <col min="10" max="11" width="10.875" style="2"/>
+    <col min="2" max="2" width="18.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.8984375" style="1"/>
+    <col min="10" max="11" width="10.8984375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +465,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -494,7 +500,7 @@
         <v>110.70347222222335</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -529,7 +535,7 @@
         <v>146.69305555555911</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -564,7 +570,7 @@
         <v>134.65277777778101</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -599,7 +605,7 @@
         <v>102.2993055555562</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -634,7 +640,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -669,7 +675,7 @@
         <v>84.541666666664241</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -704,7 +710,7 @@
         <v>78.722916666665697</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -739,7 +745,7 @@
         <v>96.727083333331393</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -774,7 +780,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -809,7 +815,7 @@
         <v>124.2770833333343</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -844,7 +850,7 @@
         <v>78.710416666668607</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -879,7 +885,7 @@
         <v>72.716666666667152</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -914,7 +920,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -949,7 +955,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -984,7 +990,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1019,7 +1025,7 @@
         <v>111.73333333332994</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>92.712500000001455</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1089,7 +1095,7 @@
         <v>80.731944444443798</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1124,7 +1130,7 @@
         <v>91.734722222223354</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1159,7 +1165,7 @@
         <v>99.715972222220444</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1194,7 +1200,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1229,7 +1235,7 @@
         <v>84.72013888888614</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1264,7 +1270,7 @@
         <v>85.730555555557657</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1299,7 +1305,7 @@
         <v>93.413888888891961</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1334,7 +1340,7 @@
         <v>95.740277777775191</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1369,7 +1375,7 @@
         <v>124.32083333333139</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1404,7 +1410,7 @@
         <v>89.75</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1439,7 +1445,7 @@
         <v>114.0402777777781</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1474,7 +1480,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1509,7 +1515,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1579,7 +1585,7 @@
         <v>101.5847222222219</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1614,7 +1620,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1649,7 +1655,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1684,7 +1690,7 @@
         <v>56.718055555553292</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1719,7 +1725,7 @@
         <v>100.72708333333139</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1754,7 +1760,7 @@
         <v>94.681250000001455</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1789,7 +1795,7 @@
         <v>59.036805555559113</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1824,7 +1830,7 @@
         <v>90.698611111110949</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1859,7 +1865,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1894,7 +1900,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1929,7 +1935,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1964,7 +1970,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1999,7 +2005,7 @@
         <v>79.726388888891961</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2034,7 +2040,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2069,7 +2075,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2104,7 +2110,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2139,7 +2145,7 @@
         <v>71.740277777775191</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2174,7 +2180,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2209,7 +2215,7 @@
         <v>73.73124999999709</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2244,7 +2250,7 @@
         <v>87.645138888889051</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2279,7 +2285,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2314,7 +2320,7 @@
         <v>107.2854166666657</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2349,7 +2355,7 @@
         <v>99.731944444443798</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2384,7 +2390,7 @@
         <v>117.73402777777665</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2419,7 +2425,7 @@
         <v>84.75</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2454,7 +2460,7 @@
         <v>78.665277777778101</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2489,7 +2495,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2524,7 +2530,7 @@
         <v>98.602777777778101</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2559,7 +2565,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2594,7 +2600,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2629,7 +2635,7 @@
         <v>97.527083333334303</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2670,15 +2676,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D46BF87884C1DD40A1748DAF71C7A50F" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9926d535f9ca60e2360c957f08e7f77f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d843a88a-8bb8-4cc6-837f-90a84e51ff60" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bc5a4ab7d3e2b3a036afd6e6a8a473c6" ns2:_="">
     <xsd:import namespace="d843a88a-8bb8-4cc6-837f-90a84e51ff60"/>
@@ -2816,6 +2813,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2827,14 +2833,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BABFB4D-DCD5-4DF1-B713-2D6886184474}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B8958E3-2AB8-4034-9E28-C0AAC35788BA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2848,6 +2846,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BABFB4D-DCD5-4DF1-B713-2D6886184474}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>